<commit_message>
add contingency table and histogram for main route
</commit_message>
<xml_diff>
--- a/data/main_routes.xlsx
+++ b/data/main_routes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EEC06D-177D-4E66-B422-5C34C7B25020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF5A79F-2CD4-4B03-B5ED-4EEA54DF9074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -626,5 +626,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>